<commit_message>
renovate wps - part
</commit_message>
<xml_diff>
--- a/CANAL/Sceleton_PUBLIC.xlsx
+++ b/CANAL/Sceleton_PUBLIC.xlsx
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>